<commit_message>
Converted whole project to keywords, for pip install and use
</commit_message>
<xml_diff>
--- a/tests/Resolutions.xlsx
+++ b/tests/Resolutions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharajaw\PycharmProjects\RF_Personal\TestSuites\Visual_UI_Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharajaw\PycharmProjects\ImageComparator\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD754E4-19CD-4A21-9D79-191406CAC4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05427634-9A32-4E44-881F-2D9BA4944A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Run</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Figma File Name</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
   <si>
     <t>Mobile</t>
@@ -417,18 +414,18 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,98 +436,95 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>